<commit_message>
modified:   "chain_data/ 	modified:   "chain_data/ 	new file:   "chain_data/ 	new file:   "chain_data/ 	new file:   "chain_data/
</commit_message>
<xml_diff>
--- a/chain_data/集成电路-基金一张网/集成电路-基金一张网20231010V1.1.xlsx
+++ b/chain_data/集成电路-基金一张网/集成电路-基金一张网20231010V1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19180" windowHeight="8200"/>
+    <workbookView windowWidth="19200" windowHeight="17800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="231">
   <si>
     <t>node_code</t>
   </si>
@@ -44,6 +44,18 @@
     <t>keyword</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>category</t>
+    </r>
+  </si>
+  <si>
     <t>03401</t>
   </si>
   <si>
@@ -80,13 +92,16 @@
     <t>集成电路制造材料，芯片制造材料，IC制造材料</t>
   </si>
   <si>
+    <t>industry_l1_name in  ('制造业','科学研究和技术服务')</t>
+  </si>
+  <si>
     <t>0340102</t>
   </si>
   <si>
     <t>封装材料</t>
   </si>
   <si>
-    <t>集成电路封装材料，芯片集成电路制，IC芯片封装材料</t>
+    <t>集成电路封装材料，芯片集成电路材料，IC芯片封装材料</t>
   </si>
   <si>
     <t>0340103</t>
@@ -131,6 +146,9 @@
     <t>新能源应用</t>
   </si>
   <si>
+    <t>industry_l1_name not in  ('批发和零售业')</t>
+  </si>
+  <si>
     <t>0340302</t>
   </si>
   <si>
@@ -279,6 +297,9 @@
   </si>
   <si>
     <t>数字集成电路设计，数字芯片设计，数字IC设计</t>
+  </si>
+  <si>
+    <t>industry_l1_name in  ('制造业','科学研究和技术服务','信息传输、软件和信息技术服务业')</t>
   </si>
   <si>
     <t>034010402</t>
@@ -720,7 +741,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,6 +760,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -887,12 +915,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1235,55 +1269,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1298,80 +1329,90 @@
     <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1719,22 +1760,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
   <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="12.9090909090909" customWidth="1"/>
     <col min="3" max="3" width="16.4545454545455" customWidth="1"/>
     <col min="4" max="4" width="20.1818181818182" customWidth="1"/>
     <col min="5" max="5" width="26.3636363636364" customWidth="1"/>
     <col min="6" max="6" width="52.2727272727273" customWidth="1"/>
+    <col min="7" max="7" width="25.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="2:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,6 +1792,9 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1756,16 +1802,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1773,16 +1819,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1790,1896 +1836,2178 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>24</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>27</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>30</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>33</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>35</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>38</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>42</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>44</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>46</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>49</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>51</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>53</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>55</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>57</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>65</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>69</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>71</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>73</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>75</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>77</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>79</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>81</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>83</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>86</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>90</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>92</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>95</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>98</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E40" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E41" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>103</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E42" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>106</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>108</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E44" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>110</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E45" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>112</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D46" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>114</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D47" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E47" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F47" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>116</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D48" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E48" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F48" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>118</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>120</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C50" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E50" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F50" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>122</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E51" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>125</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E52" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F52" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>127</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C53" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E53" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F53" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>129</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D54" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F54" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>131</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C55" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D55" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E55" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F55" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>133</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C56" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E56" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F56" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>135</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C57" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F57" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>137</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C58" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D58" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E58" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F58" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>139</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C59" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D59" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E59" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F59" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>141</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E60" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F60" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>143</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D61" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E61" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F61" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+        <v>145</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C62" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D62" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E62" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>148</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D63" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E63" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F63" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>151</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D64" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E64" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F64" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>154</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F65" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>156</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C66" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E66" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F66" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>158</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C67" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D67" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E67" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F67" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>160</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D68" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E68" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F68" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <v>163</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C69" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E69" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F69" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>165</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C70" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D70" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E70" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F70" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>167</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C71" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D71" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E71" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F71" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <v>169</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C72" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D72" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E72" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F72" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C73" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D73" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E73" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F73" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+        <v>174</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C74" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D74" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E74" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F74" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>176</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C75" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D75" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E75" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F75" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>178</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C76" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E76" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F76" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+        <v>180</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C77" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D77" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E77" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F77" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <v>182</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C78" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D78" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E78" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F78" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+        <v>184</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C79" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D79" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E79" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F79" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+        <v>186</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C80" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D80" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E80" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F80" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>188</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C81" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D81" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E81" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F81" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>191</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C82" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D82" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E82" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F82" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>193</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C83" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D83" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E83" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F83" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>195</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C84" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D84" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E84" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F84" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>198</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C85" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D85" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E85" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F85" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>201</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C86" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D86" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E86" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="F86" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>204</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C87" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D87" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E87" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F87" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>206</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C88" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D88" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E88" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F88" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+        <v>209</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C89" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D89" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E89" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F89" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+        <v>211</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C90" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D90" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E90" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F90" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+        <v>214</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C91" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D91" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E91" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F91" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <v>216</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
+        <v>217</v>
+      </c>
+      <c r="C92" t="s">
+        <v>124</v>
+      </c>
+      <c r="D92" t="s">
         <v>213</v>
       </c>
-      <c r="C92" t="s">
-        <v>120</v>
-      </c>
-      <c r="D92" t="s">
-        <v>209</v>
-      </c>
       <c r="E92" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="F92" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+        <v>218</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C93" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D93" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E93" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F93" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+        <v>220</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C94" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D94" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E94" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F94" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <v>222</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C95" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D95" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E95" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F95" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <v>224</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C96" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D96" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E96" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F96" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+        <v>226</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C97" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D97" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E97" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F97" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+        <v>228</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C98" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D98" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E98" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F98" t="s">
-        <v>226</v>
+        <v>230</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>